<commit_message>
add single data operation
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\python\python_git\python-analysis\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="80" windowWidth="16290" windowHeight="6600"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="16290" windowHeight="6600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>bdpc</t>
   </si>
@@ -156,6 +161,74 @@
   </si>
   <si>
     <t>vds</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jsd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":3}}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":4}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":5}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":6}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":8}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":10}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":11}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":13}}</t>
+  </si>
+  <si>
+    <t>{"d2":4,"dv":{"fd":16}}</t>
+  </si>
+  <si>
+    <t>{"d2":7,"dv":{"fd":12}}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d2":3,"dv":{"fd":7}}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d1":4,"dv":{"fd":9}}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d2":4}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fasdf</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>f234</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d1":4,"dv":{"fd":20}}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"d1":32,"dv":{"fm":15}}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -164,7 +237,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -757,29 +830,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -794,15 +867,15 @@
     <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -819,7 +892,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -861,7 +934,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -896,7 +969,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1105,18 +1178,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>27</v>
       </c>
@@ -1138,8 +1212,14 @@
       <c r="H1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1164,8 +1244,14 @@
       <c r="H2">
         <v>423</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I2" s="1">
+        <v>43074.043761516201</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1190,8 +1276,14 @@
       <c r="H3">
         <v>1234</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1">
+        <v>43075.043761516201</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1216,8 +1308,14 @@
       <c r="H4">
         <v>1234</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I4" s="1">
+        <v>43076.043761516201</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1242,8 +1340,14 @@
       <c r="H5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I5" s="1">
+        <v>43077.043761516201</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1268,8 +1372,14 @@
       <c r="H6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I6" s="1">
+        <v>43078.043761516201</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1294,8 +1404,14 @@
       <c r="H7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I7" s="1">
+        <v>43079.043761516201</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1317,8 +1433,14 @@
       <c r="H8">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I8" s="1">
+        <v>43080.043761516201</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1337,8 +1459,14 @@
       <c r="H9">
         <v>5364</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I9" s="1">
+        <v>43081.043761458335</v>
+      </c>
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1363,8 +1491,14 @@
       <c r="H10">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="I10" s="1">
+        <v>43082.043761458335</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1389,8 +1523,14 @@
       <c r="H11">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>43076.043761516201</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1409,8 +1549,14 @@
       <c r="H12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>43077.043761516201</v>
+      </c>
+      <c r="J12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1429,8 +1575,14 @@
       <c r="G13" s="1">
         <v>43081.043761458335</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1">
+        <v>43078.043761516201</v>
+      </c>
+      <c r="J13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1455,8 +1607,14 @@
       <c r="H14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1">
+        <v>43079.043761516201</v>
+      </c>
+      <c r="J14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1478,8 +1636,14 @@
       <c r="H15">
         <v>134</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <v>43080.043761516201</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1504,8 +1668,14 @@
       <c r="H16">
         <v>5364</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <v>43074.043761516201</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1530,8 +1700,11 @@
       <c r="H17">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>43075.043761516201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1556,8 +1729,14 @@
       <c r="H18">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <v>43076.043761516201</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1579,8 +1758,14 @@
       <c r="H19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>43077.043761516201</v>
+      </c>
+      <c r="J19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1599,6 +1784,18 @@
       <c r="G20" s="1">
         <v>43088.043761458335</v>
       </c>
+      <c r="I20" s="1">
+        <v>43078.043761516201</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I22" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
use multiprocess for data processing
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>bdpc</t>
   </si>
@@ -116,10 +116,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>C</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>G</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -132,10 +128,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>HIS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>a</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -229,6 +221,22 @@
   </si>
   <si>
     <t>{"d1":32,"dv":{"fm":15}}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文列测试</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdg,dasf,fas</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ngfsg,qewr</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1181,7 +1189,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1198,25 +1206,25 @@
         <v>28</v>
       </c>
       <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
@@ -1248,7 +1256,7 @@
         <v>43074.043761516201</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -1280,7 +1288,7 @@
         <v>43075.043761516201</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -1312,7 +1320,7 @@
         <v>43076.043761516201</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
@@ -1344,7 +1352,7 @@
         <v>43077.043761516201</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -1376,7 +1384,7 @@
         <v>43078.043761516201</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -1408,7 +1416,7 @@
         <v>43079.043761516201</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
@@ -1437,7 +1445,7 @@
         <v>43080.043761516201</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
@@ -1463,7 +1471,7 @@
         <v>43081.043761458335</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
@@ -1474,7 +1482,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1495,7 +1503,7 @@
         <v>43082.043761458335</v>
       </c>
       <c r="J10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
@@ -1527,7 +1535,7 @@
         <v>43076.043761516201</v>
       </c>
       <c r="J11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -1553,7 +1561,7 @@
         <v>43077.043761516201</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
@@ -1561,7 +1569,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1579,7 +1587,7 @@
         <v>43078.043761516201</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
@@ -1587,13 +1595,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -1605,13 +1613,11 @@
         <v>43082.043761458335</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="1">
-        <v>43079.043761516201</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I14" s="1"/>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
@@ -1622,7 +1628,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
@@ -1640,7 +1646,7 @@
         <v>43080.043761516201</v>
       </c>
       <c r="J15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
@@ -1651,7 +1657,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
@@ -1672,7 +1678,7 @@
         <v>43074.043761516201</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
@@ -1733,7 +1739,7 @@
         <v>43076.043761516201</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
@@ -1744,7 +1750,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -1762,7 +1768,7 @@
         <v>43077.043761516201</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
@@ -1770,7 +1776,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
parsejson option can parse array
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\python\python_git\python-analysis\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="16290" windowHeight="6600"/>
+    <workbookView xWindow="480" yWindow="80" windowWidth="16290" windowHeight="6600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>bdpc</t>
   </si>
@@ -237,6 +232,72 @@
   </si>
   <si>
     <t>ngfsg,qewr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jsa</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"ds":3}</t>
+  </si>
+  <si>
+    <t>{"ds":4}</t>
+  </si>
+  <si>
+    <t>[1,3,2]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1,3,3]</t>
+  </si>
+  <si>
+    <t>[1,3,4]</t>
+  </si>
+  <si>
+    <t>["21",3,5]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>["21",3,6]</t>
+  </si>
+  <si>
+    <t>["21",3,"123"]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>["21",3,"124"]</t>
+  </si>
+  <si>
+    <t>["21",3,"125"]</t>
+  </si>
+  <si>
+    <t>["22","ds","ase"]</t>
+  </si>
+  <si>
+    <t>{"a":["23","ds","ase"]}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"a":["24","ds","ase"],"b":1}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"a":["24","ds","ase"],"b":2}</t>
+  </si>
+  <si>
+    <t>{"a":["24","ds","ase"],"b":3}</t>
+  </si>
+  <si>
+    <t>[[12,33,11],"ds","ase"]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>["21",{"wq":"re"},"126"]</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -843,24 +904,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -875,15 +936,15 @@
     <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -900,7 +961,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -942,7 +1003,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,7 +1038,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1186,19 +1247,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>27</v>
       </c>
@@ -1226,8 +1287,11 @@
       <c r="J1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1258,8 +1322,11 @@
       <c r="J2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1290,8 +1357,11 @@
       <c r="J3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1322,8 +1392,11 @@
       <c r="J4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1354,8 +1427,11 @@
       <c r="J5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1386,8 +1462,11 @@
       <c r="J6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1403,8 +1482,8 @@
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>6.9444444440000002</v>
+      <c r="F7" t="s">
+        <v>62</v>
       </c>
       <c r="G7" s="1">
         <v>43075.043761516201</v>
@@ -1418,8 +1497,11 @@
       <c r="J7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1447,8 +1529,11 @@
       <c r="J8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1473,8 +1558,11 @@
       <c r="J9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1505,8 +1593,11 @@
       <c r="J10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1537,8 +1628,11 @@
       <c r="J11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1548,9 +1642,6 @@
       <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="F12">
-        <v>7.777777779</v>
-      </c>
       <c r="G12" s="1">
         <v>43080.043761516201</v>
       </c>
@@ -1563,8 +1654,11 @@
       <c r="J12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1589,8 +1683,11 @@
       <c r="J13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1619,8 +1716,11 @@
       <c r="J14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1648,8 +1748,11 @@
       <c r="J15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1680,8 +1783,11 @@
       <c r="J16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1697,9 +1803,6 @@
       <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17">
-        <v>7.4444444440000002</v>
-      </c>
       <c r="G17" s="1">
         <v>43085.043761458335</v>
       </c>
@@ -1709,8 +1812,11 @@
       <c r="I17" s="1">
         <v>43075.043761516201</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1741,8 +1847,11 @@
       <c r="J18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1771,7 +1880,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1796,11 +1905,14 @@
       <c r="J20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" ht="13.5" x14ac:dyDescent="0.15">
       <c r="I22" s="1"/>
     </row>
   </sheetData>

</xml_diff>